<commit_message>
Change in the milestone name for " Meeting with proponent\
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/amendment/002_Amendment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/amendment/002_Amendment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FF67AC-EFAD-4A17-BA21-4BDCE3A82A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67577617-A489-4E8D-B9B5-BD17B937BC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="259">
   <si>
     <t>No</t>
   </si>
@@ -821,6 +821,9 @@
   </si>
   <si>
     <t>[{"phase_name":"Amendment Review (Typical)","work_type_id": 7, "ea_act_id": 3, "is_active": false }]</t>
+  </si>
+  <si>
+    <t>Initial Meeting with Proponent</t>
   </si>
 </sst>
 </file>
@@ -2336,11 +2339,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M347"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D161" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L115" sqref="L115"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -2445,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>141</v>
+        <v>258</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>IF((C3=""),"",VLOOKUP(C3,Phases!$A$2:$B$10,2,FALSE))</f>
@@ -14420,8 +14423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
@@ -19131,14 +19134,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19371,21 +19372,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19410,9 +19410,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change in the milestone name for " Meeting with proponent\ (#2322)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/amendment/002_Amendment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/amendment/002_Amendment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\amendment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FF67AC-EFAD-4A17-BA21-4BDCE3A82A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67577617-A489-4E8D-B9B5-BD17B937BC91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="259">
   <si>
     <t>No</t>
   </si>
@@ -821,6 +821,9 @@
   </si>
   <si>
     <t>[{"phase_name":"Amendment Review (Typical)","work_type_id": 7, "ea_act_id": 3, "is_active": false }]</t>
+  </si>
+  <si>
+    <t>Initial Meeting with Proponent</t>
   </si>
 </sst>
 </file>
@@ -2336,11 +2339,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M347"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D161" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L115" sqref="L115"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -2445,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>141</v>
+        <v>258</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>IF((C3=""),"",VLOOKUP(C3,Phases!$A$2:$B$10,2,FALSE))</f>
@@ -14420,8 +14423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
@@ -19131,14 +19134,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19371,21 +19372,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19410,9 +19410,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>